<commit_message>
Update to add region
</commit_message>
<xml_diff>
--- a/MultisysBOM_Options.xlsx
+++ b/MultisysBOM_Options.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petermcclelland/Desktop/track_1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petermcclelland/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD58E215-9B1E-194C-B9D4-1A6B0463F45A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3529C318-62D0-CF48-95B0-F0F7F367154D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9080" yWindow="11920" windowWidth="24520" windowHeight="7680" activeTab="1" xr2:uid="{984AE996-C24A-134E-92AC-58AF8C1B965D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{984AE996-C24A-134E-92AC-58AF8C1B965D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="67">
   <si>
     <t>Type</t>
   </si>
@@ -199,6 +199,45 @@
   </si>
   <si>
     <t>RBKTRL-01</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Metric</t>
+  </si>
+  <si>
+    <t>Imperial</t>
+  </si>
+  <si>
+    <t>ST1-9500-4FT-**</t>
+  </si>
+  <si>
+    <t>ST8-9500-4FT-**</t>
+  </si>
+  <si>
+    <t>ST3-9500-4FT-**</t>
+  </si>
+  <si>
+    <t>ST6-9500-4FT-**</t>
+  </si>
+  <si>
+    <t>ST1-9500-8FT-**</t>
+  </si>
+  <si>
+    <t>ST8-9500-8FT-**</t>
+  </si>
+  <si>
+    <t>ST3-9500-8FT-**</t>
+  </si>
+  <si>
+    <t>ST6-9500-8FT-**</t>
+  </si>
+  <si>
+    <t>Imperial 4ft</t>
+  </si>
+  <si>
+    <t>Imperial 8ft</t>
   </si>
 </sst>
 </file>
@@ -576,23 +615,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{230DE009-48E9-DC46-84A9-3CD49F909332}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" customWidth="1"/>
+    <col min="4" max="4" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -600,19 +640,22 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -620,19 +663,22 @@
         <v>20</v>
       </c>
       <c r="C2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" t="s">
         <v>24</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>26</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>28</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -640,219 +686,268 @@
         <v>20</v>
       </c>
       <c r="C3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" t="s">
         <v>25</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>27</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>29</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
       </c>
-      <c r="C6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
       </c>
-      <c r="C7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>12</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
       </c>
-      <c r="C11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
       </c>
-      <c r="C12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" t="s">
-        <v>40</v>
-      </c>
-      <c r="F14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" t="s">
-        <v>41</v>
-      </c>
-      <c r="F15" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>16</v>
       </c>
       <c r="B16" t="s">
         <v>9</v>
       </c>
-      <c r="C16" t="s">
-        <v>42</v>
-      </c>
       <c r="D16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="G16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>9</v>
       </c>
-      <c r="C17" t="s">
-        <v>43</v>
-      </c>
       <c r="D17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F17" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="G17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
         <v>9</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" t="s">
+        <v>43</v>
+      </c>
+      <c r="G19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" t="s">
         <v>44</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E20" t="s">
         <v>44</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F20" t="s">
         <v>44</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G20" t="s">
         <v>44</v>
       </c>
     </row>
@@ -866,7 +961,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43C97794-5515-DF4A-A116-1E56A2431733}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>